<commit_message>
Cambios generales de formulario pedidos, inventario, planilla y viajes, junto a al historia de ventas
</commit_message>
<xml_diff>
--- a/ProyectoPooDist/excels/clientes.xlsx
+++ b/ProyectoPooDist/excels/clientes.xlsx
@@ -154,6 +154,12 @@
       <c r="D4" t="n" s="0">
         <v>1.0</v>
       </c>
+      <c r="E4" t="n" s="0">
+        <v>4.0</v>
+      </c>
+      <c r="F4" t="n" s="0">
+        <v>5.0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
@@ -180,10 +186,28 @@
       <c r="H5" t="n" s="0">
         <v>198.0</v>
       </c>
+      <c r="I5" t="n" s="0">
+        <v>7.0</v>
+      </c>
+      <c r="J5" t="n" s="0">
+        <v>150.0</v>
+      </c>
     </row>
     <row r="6">
       <c r="C6" t="n" s="0">
         <v>2.0</v>
+      </c>
+      <c r="D6" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="E6" t="n" s="0">
+        <v>6.0</v>
+      </c>
+      <c r="F6" t="n" s="0">
+        <v>7.0</v>
+      </c>
+      <c r="G6" t="n" s="0">
+        <v>8.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SOLUCION DE CONFLICTOS ENTRE LAS GESTIONES: CALENDARIO - PEDIDO - CAMIONES - PILOTOS
</commit_message>
<xml_diff>
--- a/ProyectoPooDist/excels/clientes.xlsx
+++ b/ProyectoPooDist/excels/clientes.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>Clientes Varios</t>
   </si>
@@ -101,6 +101,12 @@
   <si>
     <t>Cliente mayorista de lactomayma 
 y lactomayma 22 porciento</t>
+  </si>
+  <si>
+    <t>José González</t>
+  </si>
+  <si>
+    <t>Patrocinador Oficial de Distribuidora PINE</t>
   </si>
 </sst>
 </file>
@@ -145,7 +151,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AB30"/>
+  <dimension ref="A1:AB32"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -567,6 +573,15 @@
         <v>21.0</v>
       </c>
     </row>
+    <row r="31">
+      <c r="A31" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="B31" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32"/>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>